<commit_message>
updateing data analysis stuff
</commit_message>
<xml_diff>
--- a/Tests/MATLAB/Vincent/flow sensor/txt data/final data.xlsx
+++ b/Tests/MATLAB/Vincent/flow sensor/txt data/final data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vinst\Documents\school(uni)\year_3\final year project\experiments\flow sensor\txt data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870ED41C-A20E-4483-8B1C-C02AFAF9FFF6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A45E838-D841-40DF-806F-FF1EC6221C0B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" tabRatio="689" xr2:uid="{7EA9EAC3-4B90-479D-BAFE-81A752B1E75B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" tabRatio="689" activeTab="5" xr2:uid="{7EA9EAC3-4B90-479D-BAFE-81A752B1E75B}"/>
   </bookViews>
   <sheets>
     <sheet name="hum0G50psivis" sheetId="1" r:id="rId1"/>
@@ -376,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EC59F9-F0B1-4D29-A289-BA516BFA5988}">
-  <dimension ref="A1:X88"/>
+  <dimension ref="A1:W89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:X88"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1304,7 +1304,7 @@
         <v>1323034</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>239</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>1341971</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>239</v>
       </c>
@@ -1389,7 +1389,7 @@
         <v>1383215</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>108428</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>1394786</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>239</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>1466577</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>239</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>1443192</v>
       </c>
       <c r="I21">
-        <v>36532248</v>
+        <v>248</v>
       </c>
       <c r="J21">
         <v>367</v>
@@ -1532,9 +1532,6 @@
       <c r="O21">
         <v>1718105</v>
       </c>
-      <c r="P21">
-        <v>1718176</v>
-      </c>
       <c r="Q21">
         <v>89348</v>
       </c>
@@ -1542,7 +1539,7 @@
         <v>1472711</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>127728</v>
       </c>
@@ -1550,25 +1547,10 @@
         <v>1456587</v>
       </c>
       <c r="I22">
-        <v>248</v>
+        <v>36532</v>
       </c>
       <c r="J22">
-        <v>368</v>
-      </c>
-      <c r="K22">
-        <v>346</v>
-      </c>
-      <c r="L22">
-        <v>574</v>
-      </c>
-      <c r="M22">
-        <v>431</v>
-      </c>
-      <c r="N22">
-        <v>390</v>
-      </c>
-      <c r="O22">
-        <v>1789853</v>
+        <v>1718176</v>
       </c>
       <c r="Q22">
         <v>31720</v>
@@ -1577,7 +1559,7 @@
         <v>1504473</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>37356</v>
       </c>
@@ -1585,10 +1567,25 @@
         <v>1493707</v>
       </c>
       <c r="I23">
-        <v>80940</v>
+        <v>248</v>
       </c>
       <c r="J23">
-        <v>1799157</v>
+        <v>368</v>
+      </c>
+      <c r="K23">
+        <v>346</v>
+      </c>
+      <c r="L23">
+        <v>574</v>
+      </c>
+      <c r="M23">
+        <v>431</v>
+      </c>
+      <c r="N23">
+        <v>390</v>
+      </c>
+      <c r="O23">
+        <v>1789853</v>
       </c>
       <c r="Q23">
         <v>247</v>
@@ -1612,7 +1609,7 @@
         <v>1538283</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>239</v>
       </c>
@@ -1635,10 +1632,10 @@
         <v>1514943</v>
       </c>
       <c r="I24">
-        <v>29012</v>
+        <v>80940</v>
       </c>
       <c r="J24">
-        <v>1828218</v>
+        <v>1799157</v>
       </c>
       <c r="Q24">
         <v>85656</v>
@@ -1647,7 +1644,7 @@
         <v>1590269</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>239</v>
       </c>
@@ -1670,25 +1667,10 @@
         <v>1586736</v>
       </c>
       <c r="I25">
-        <v>248</v>
+        <v>29012</v>
       </c>
       <c r="J25">
-        <v>368</v>
-      </c>
-      <c r="K25">
-        <v>346</v>
-      </c>
-      <c r="L25">
-        <v>574</v>
-      </c>
-      <c r="M25">
-        <v>431</v>
-      </c>
-      <c r="N25">
-        <v>390</v>
-      </c>
-      <c r="O25">
-        <v>1861642</v>
+        <v>1828218</v>
       </c>
       <c r="Q25">
         <v>247</v>
@@ -1712,7 +1694,7 @@
         <v>1610035</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>94184</v>
       </c>
@@ -1720,10 +1702,25 @@
         <v>1588038</v>
       </c>
       <c r="I26">
-        <v>78496</v>
+        <v>248</v>
       </c>
       <c r="J26">
-        <v>1906843</v>
+        <v>368</v>
+      </c>
+      <c r="K26">
+        <v>346</v>
+      </c>
+      <c r="L26">
+        <v>574</v>
+      </c>
+      <c r="M26">
+        <v>431</v>
+      </c>
+      <c r="N26">
+        <v>390</v>
+      </c>
+      <c r="O26">
+        <v>1861642</v>
       </c>
       <c r="Q26">
         <v>34620</v>
@@ -1732,7 +1729,7 @@
         <v>1624944</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>35736</v>
       </c>
@@ -1740,25 +1737,10 @@
         <v>1623833</v>
       </c>
       <c r="I27">
-        <v>248</v>
+        <v>78496</v>
       </c>
       <c r="J27">
-        <v>368</v>
-      </c>
-      <c r="K27">
-        <v>345</v>
-      </c>
-      <c r="L27">
-        <v>574</v>
-      </c>
-      <c r="M27">
-        <v>432</v>
-      </c>
-      <c r="N27">
-        <v>390</v>
-      </c>
-      <c r="O27">
-        <v>1933349</v>
+        <v>1906843</v>
       </c>
       <c r="Q27">
         <v>247</v>
@@ -1782,7 +1764,7 @@
         <v>1681785</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>239</v>
       </c>
@@ -1805,10 +1787,25 @@
         <v>1658439</v>
       </c>
       <c r="I28">
-        <v>31792</v>
+        <v>248</v>
       </c>
       <c r="J28">
-        <v>1938687</v>
+        <v>368</v>
+      </c>
+      <c r="K28">
+        <v>345</v>
+      </c>
+      <c r="L28">
+        <v>574</v>
+      </c>
+      <c r="M28">
+        <v>432</v>
+      </c>
+      <c r="N28">
+        <v>390</v>
+      </c>
+      <c r="O28">
+        <v>1933349</v>
       </c>
       <c r="Q28">
         <v>81296</v>
@@ -1817,7 +1814,7 @@
         <v>1706368</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>83000</v>
       </c>
@@ -1825,25 +1822,10 @@
         <v>1706962</v>
       </c>
       <c r="I29">
-        <v>248</v>
+        <v>31792</v>
       </c>
       <c r="J29">
-        <v>368</v>
-      </c>
-      <c r="K29">
-        <v>345</v>
-      </c>
-      <c r="L29">
-        <v>574</v>
-      </c>
-      <c r="M29">
-        <v>431</v>
-      </c>
-      <c r="N29">
-        <v>390</v>
-      </c>
-      <c r="O29">
-        <v>2005101</v>
+        <v>1938687</v>
       </c>
       <c r="Q29">
         <v>30904</v>
@@ -1852,7 +1834,7 @@
         <v>1737331</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>239</v>
       </c>
@@ -1875,10 +1857,25 @@
         <v>1730191</v>
       </c>
       <c r="I30">
-        <v>75296</v>
+        <v>248</v>
       </c>
       <c r="J30">
-        <v>2014109</v>
+        <v>368</v>
+      </c>
+      <c r="K30">
+        <v>345</v>
+      </c>
+      <c r="L30">
+        <v>574</v>
+      </c>
+      <c r="M30">
+        <v>431</v>
+      </c>
+      <c r="N30">
+        <v>390</v>
+      </c>
+      <c r="O30">
+        <v>2005101</v>
       </c>
       <c r="Q30">
         <v>247</v>
@@ -1902,7 +1899,7 @@
         <v>1753576</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30464</v>
       </c>
@@ -1910,13 +1907,13 @@
         <v>1737486</v>
       </c>
       <c r="I31">
-        <v>28624</v>
+        <v>75296</v>
       </c>
       <c r="J31">
-        <v>2042773</v>
+        <v>2014109</v>
       </c>
       <c r="Q31">
-        <v>87784247</v>
+        <v>247</v>
       </c>
       <c r="R31">
         <v>367</v>
@@ -1936,11 +1933,8 @@
       <c r="W31">
         <v>1825286</v>
       </c>
-      <c r="X31">
-        <v>1825357</v>
-      </c>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>239</v>
       </c>
@@ -1963,31 +1957,16 @@
         <v>1801942</v>
       </c>
       <c r="I32">
-        <v>248</v>
+        <v>28624</v>
       </c>
       <c r="J32">
-        <v>368</v>
-      </c>
-      <c r="K32">
-        <v>345</v>
-      </c>
-      <c r="L32">
-        <v>574</v>
-      </c>
-      <c r="M32">
-        <v>431</v>
-      </c>
-      <c r="N32">
-        <v>390</v>
-      </c>
-      <c r="O32">
-        <v>2076851</v>
+        <v>2042773</v>
       </c>
       <c r="Q32">
-        <v>38588</v>
+        <v>87784</v>
       </c>
       <c r="R32">
-        <v>1863898</v>
+        <v>1825357</v>
       </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
@@ -1998,31 +1977,31 @@
         <v>1823056</v>
       </c>
       <c r="I33">
-        <v>79756</v>
+        <v>248</v>
       </c>
       <c r="J33">
-        <v>2122658</v>
+        <v>368</v>
+      </c>
+      <c r="K33">
+        <v>345</v>
+      </c>
+      <c r="L33">
+        <v>574</v>
+      </c>
+      <c r="M33">
+        <v>431</v>
+      </c>
+      <c r="N33">
+        <v>390</v>
+      </c>
+      <c r="O33">
+        <v>2076851</v>
       </c>
       <c r="Q33">
-        <v>247</v>
+        <v>38588</v>
       </c>
       <c r="R33">
-        <v>367</v>
-      </c>
-      <c r="S33">
-        <v>346</v>
-      </c>
-      <c r="T33">
-        <v>574</v>
-      </c>
-      <c r="U33">
-        <v>432</v>
-      </c>
-      <c r="V33">
-        <v>390</v>
-      </c>
-      <c r="W33">
-        <v>1897034</v>
+        <v>1863898</v>
       </c>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
@@ -2033,31 +2012,31 @@
         <v>1859595</v>
       </c>
       <c r="I34">
-        <v>248</v>
+        <v>79756</v>
       </c>
       <c r="J34">
-        <v>368</v>
-      </c>
-      <c r="K34">
-        <v>345</v>
-      </c>
-      <c r="L34">
+        <v>2122658</v>
+      </c>
+      <c r="Q34">
+        <v>247</v>
+      </c>
+      <c r="R34">
+        <v>367</v>
+      </c>
+      <c r="S34">
+        <v>346</v>
+      </c>
+      <c r="T34">
         <v>574</v>
       </c>
-      <c r="M34">
+      <c r="U34">
         <v>432</v>
       </c>
-      <c r="N34">
+      <c r="V34">
         <v>390</v>
       </c>
-      <c r="O34">
-        <v>2148641</v>
-      </c>
-      <c r="Q34">
-        <v>93424</v>
-      </c>
-      <c r="R34">
-        <v>1957474</v>
+      <c r="W34">
+        <v>1897034</v>
       </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
@@ -2083,31 +2062,31 @@
         <v>1873733</v>
       </c>
       <c r="I35">
-        <v>34040</v>
+        <v>248</v>
       </c>
       <c r="J35">
-        <v>2156761</v>
+        <v>368</v>
+      </c>
+      <c r="K35">
+        <v>345</v>
+      </c>
+      <c r="L35">
+        <v>574</v>
+      </c>
+      <c r="M35">
+        <v>432</v>
+      </c>
+      <c r="N35">
+        <v>390</v>
+      </c>
+      <c r="O35">
+        <v>2148641</v>
       </c>
       <c r="Q35">
-        <v>243</v>
+        <v>93424</v>
       </c>
       <c r="R35">
-        <v>367</v>
-      </c>
-      <c r="S35">
-        <v>339</v>
-      </c>
-      <c r="T35">
-        <v>575</v>
-      </c>
-      <c r="U35">
-        <v>431</v>
-      </c>
-      <c r="V35">
-        <v>392</v>
-      </c>
-      <c r="W35">
-        <v>1968824</v>
+        <v>1957474</v>
       </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
@@ -2133,31 +2112,31 @@
         <v>1945438</v>
       </c>
       <c r="I36">
-        <v>246</v>
+        <v>34040</v>
       </c>
       <c r="J36">
+        <v>2156761</v>
+      </c>
+      <c r="Q36">
+        <v>243</v>
+      </c>
+      <c r="R36">
         <v>367</v>
       </c>
-      <c r="K36">
-        <v>341</v>
-      </c>
-      <c r="L36">
+      <c r="S36">
+        <v>339</v>
+      </c>
+      <c r="T36">
         <v>575</v>
       </c>
-      <c r="M36">
+      <c r="U36">
         <v>431</v>
       </c>
-      <c r="N36">
+      <c r="V36">
         <v>392</v>
       </c>
-      <c r="O36">
-        <v>2220348</v>
-      </c>
-      <c r="Q36">
-        <v>38160</v>
-      </c>
-      <c r="R36">
-        <v>1995697</v>
+      <c r="W36">
+        <v>1968824</v>
       </c>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
@@ -2168,31 +2147,31 @@
         <v>1949535</v>
       </c>
       <c r="I37">
-        <v>81444</v>
+        <v>246</v>
       </c>
       <c r="J37">
-        <v>2238328</v>
+        <v>367</v>
+      </c>
+      <c r="K37">
+        <v>341</v>
+      </c>
+      <c r="L37">
+        <v>575</v>
+      </c>
+      <c r="M37">
+        <v>431</v>
+      </c>
+      <c r="N37">
+        <v>392</v>
+      </c>
+      <c r="O37">
+        <v>2220348</v>
       </c>
       <c r="Q37">
-        <v>230</v>
+        <v>38160</v>
       </c>
       <c r="R37">
-        <v>368</v>
-      </c>
-      <c r="S37">
-        <v>339</v>
-      </c>
-      <c r="T37">
-        <v>575</v>
-      </c>
-      <c r="U37">
-        <v>431</v>
-      </c>
-      <c r="V37">
-        <v>392</v>
-      </c>
-      <c r="W37">
-        <v>2040530</v>
+        <v>1995697</v>
       </c>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
@@ -2203,16 +2182,31 @@
         <v>1985357</v>
       </c>
       <c r="I38">
-        <v>32048</v>
+        <v>81444</v>
       </c>
       <c r="J38">
-        <v>2270425</v>
+        <v>2238328</v>
       </c>
       <c r="Q38">
-        <v>108972</v>
+        <v>230</v>
       </c>
       <c r="R38">
-        <v>2105140</v>
+        <v>368</v>
+      </c>
+      <c r="S38">
+        <v>339</v>
+      </c>
+      <c r="T38">
+        <v>575</v>
+      </c>
+      <c r="U38">
+        <v>431</v>
+      </c>
+      <c r="V38">
+        <v>392</v>
+      </c>
+      <c r="W38">
+        <v>2040530</v>
       </c>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
@@ -2238,131 +2232,101 @@
         <v>2017190</v>
       </c>
       <c r="I39">
-        <v>246</v>
+        <v>32048</v>
       </c>
       <c r="J39">
-        <v>367</v>
-      </c>
-      <c r="K39">
-        <v>341</v>
-      </c>
-      <c r="L39">
-        <v>575</v>
-      </c>
-      <c r="M39">
-        <v>431</v>
-      </c>
-      <c r="N39">
-        <v>392</v>
-      </c>
-      <c r="O39">
-        <v>2292101</v>
+        <v>2270425</v>
       </c>
       <c r="Q39">
-        <v>230</v>
+        <v>108972</v>
       </c>
       <c r="R39">
-        <v>368</v>
-      </c>
-      <c r="S39">
-        <v>334</v>
-      </c>
-      <c r="T39">
-        <v>572</v>
-      </c>
-      <c r="U39">
-        <v>432</v>
-      </c>
-      <c r="V39">
-        <v>391</v>
-      </c>
-      <c r="W39">
-        <v>2112281</v>
+        <v>2105140</v>
       </c>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>103044</v>
+        <v>233</v>
+      </c>
+      <c r="B40">
+        <v>369</v>
+      </c>
+      <c r="C40">
+        <v>334</v>
+      </c>
+      <c r="D40">
+        <v>569</v>
+      </c>
+      <c r="E40">
+        <v>433</v>
+      </c>
+      <c r="F40">
+        <v>392</v>
+      </c>
+      <c r="G40">
+        <v>2088983</v>
       </c>
       <c r="I40">
-        <v>91756</v>
+        <v>246</v>
       </c>
       <c r="J40">
-        <v>2362331</v>
+        <v>367</v>
+      </c>
+      <c r="K40">
+        <v>341</v>
+      </c>
+      <c r="L40">
+        <v>575</v>
+      </c>
+      <c r="M40">
+        <v>431</v>
+      </c>
+      <c r="N40">
+        <v>392</v>
+      </c>
+      <c r="O40">
+        <v>2292101</v>
       </c>
       <c r="Q40">
-        <v>50468</v>
+        <v>230</v>
       </c>
       <c r="R40">
-        <v>2155389</v>
+        <v>368</v>
+      </c>
+      <c r="S40">
+        <v>334</v>
+      </c>
+      <c r="T40">
+        <v>572</v>
+      </c>
+      <c r="U40">
+        <v>432</v>
+      </c>
+      <c r="V40">
+        <v>391</v>
+      </c>
+      <c r="W40">
+        <v>2112281</v>
       </c>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>233</v>
+        <v>103044</v>
       </c>
       <c r="B41">
-        <v>369</v>
-      </c>
-      <c r="C41">
-        <v>334</v>
-      </c>
-      <c r="D41">
-        <v>569</v>
-      </c>
-      <c r="E41">
-        <v>433</v>
-      </c>
-      <c r="F41">
-        <v>392</v>
-      </c>
-      <c r="G41">
-        <v>2088983</v>
-      </c>
-      <c r="H41">
         <v>2089049</v>
       </c>
       <c r="I41">
-        <v>239</v>
+        <v>91756</v>
       </c>
       <c r="J41">
-        <v>368</v>
-      </c>
-      <c r="K41">
-        <v>338</v>
-      </c>
-      <c r="L41">
-        <v>574</v>
-      </c>
-      <c r="M41">
-        <v>431</v>
-      </c>
-      <c r="N41">
-        <v>392</v>
-      </c>
-      <c r="O41">
-        <v>2363890</v>
+        <v>2362331</v>
       </c>
       <c r="Q41">
-        <v>186</v>
+        <v>50468</v>
       </c>
       <c r="R41">
-        <v>366</v>
-      </c>
-      <c r="S41">
-        <v>309</v>
-      </c>
-      <c r="T41">
-        <v>559</v>
-      </c>
-      <c r="U41">
-        <v>431</v>
-      </c>
-      <c r="V41">
-        <v>388</v>
-      </c>
-      <c r="W41">
-        <v>2184073</v>
+        <v>2155389</v>
       </c>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
@@ -2373,10 +2337,25 @@
         <v>2135262</v>
       </c>
       <c r="I42">
-        <v>40816</v>
+        <v>239</v>
       </c>
       <c r="J42">
-        <v>2403213</v>
+        <v>368</v>
+      </c>
+      <c r="K42">
+        <v>338</v>
+      </c>
+      <c r="L42">
+        <v>574</v>
+      </c>
+      <c r="M42">
+        <v>431</v>
+      </c>
+      <c r="N42">
+        <v>392</v>
+      </c>
+      <c r="O42">
+        <v>2363890</v>
       </c>
       <c r="Q42">
         <v>186</v>
@@ -2397,7 +2376,7 @@
         <v>388</v>
       </c>
       <c r="W42">
-        <v>2255777</v>
+        <v>2184073</v>
       </c>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
@@ -2423,31 +2402,31 @@
         <v>2160687</v>
       </c>
       <c r="I43">
-        <v>214</v>
+        <v>40816</v>
       </c>
       <c r="J43">
-        <v>368</v>
-      </c>
-      <c r="K43">
-        <v>325</v>
-      </c>
-      <c r="L43">
-        <v>568</v>
-      </c>
-      <c r="M43">
+        <v>2403213</v>
+      </c>
+      <c r="Q43">
+        <v>186</v>
+      </c>
+      <c r="R43">
+        <v>366</v>
+      </c>
+      <c r="S43">
+        <v>309</v>
+      </c>
+      <c r="T43">
+        <v>559</v>
+      </c>
+      <c r="U43">
         <v>431</v>
       </c>
-      <c r="N43">
-        <v>392</v>
-      </c>
-      <c r="O43">
-        <v>2435597</v>
-      </c>
-      <c r="Q43">
-        <v>122892</v>
-      </c>
-      <c r="R43">
-        <v>2278773</v>
+      <c r="V43">
+        <v>388</v>
+      </c>
+      <c r="W43">
+        <v>2255777</v>
       </c>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
@@ -2473,31 +2452,31 @@
         <v>2232439</v>
       </c>
       <c r="I44">
-        <v>98428</v>
+        <v>214</v>
       </c>
       <c r="J44">
-        <v>2501796</v>
+        <v>368</v>
+      </c>
+      <c r="K44">
+        <v>325</v>
+      </c>
+      <c r="L44">
+        <v>568</v>
+      </c>
+      <c r="M44">
+        <v>431</v>
+      </c>
+      <c r="N44">
+        <v>392</v>
+      </c>
+      <c r="O44">
+        <v>2435597</v>
       </c>
       <c r="Q44">
-        <v>159</v>
+        <v>122892</v>
       </c>
       <c r="R44">
-        <v>363</v>
-      </c>
-      <c r="S44">
-        <v>294</v>
-      </c>
-      <c r="T44">
-        <v>545</v>
-      </c>
-      <c r="U44">
-        <v>432</v>
-      </c>
-      <c r="V44">
-        <v>383</v>
-      </c>
-      <c r="W44">
-        <v>2327528</v>
+        <v>2278773</v>
       </c>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
@@ -2508,31 +2487,31 @@
         <v>2249637</v>
       </c>
       <c r="I45">
-        <v>214</v>
+        <v>98428</v>
       </c>
       <c r="J45">
-        <v>368</v>
-      </c>
-      <c r="K45">
-        <v>325</v>
-      </c>
-      <c r="L45">
-        <v>568</v>
-      </c>
-      <c r="M45">
+        <v>2501796</v>
+      </c>
+      <c r="Q45">
+        <v>159</v>
+      </c>
+      <c r="R45">
+        <v>363</v>
+      </c>
+      <c r="S45">
+        <v>294</v>
+      </c>
+      <c r="T45">
+        <v>545</v>
+      </c>
+      <c r="U45">
         <v>432</v>
       </c>
-      <c r="N45">
-        <v>390</v>
-      </c>
-      <c r="O45">
-        <v>2507346</v>
-      </c>
-      <c r="Q45">
-        <v>54240</v>
-      </c>
-      <c r="R45">
-        <v>2332804</v>
+      <c r="V45">
+        <v>383</v>
+      </c>
+      <c r="W45">
+        <v>2327528</v>
       </c>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
@@ -2543,31 +2522,31 @@
         <v>2297967</v>
       </c>
       <c r="I46">
-        <v>41080</v>
+        <v>214</v>
       </c>
       <c r="J46">
-        <v>2542945</v>
+        <v>368</v>
+      </c>
+      <c r="K46">
+        <v>325</v>
+      </c>
+      <c r="L46">
+        <v>568</v>
+      </c>
+      <c r="M46">
+        <v>432</v>
+      </c>
+      <c r="N46">
+        <v>390</v>
+      </c>
+      <c r="O46">
+        <v>2507346</v>
       </c>
       <c r="Q46">
-        <v>128</v>
+        <v>54240</v>
       </c>
       <c r="R46">
-        <v>356</v>
-      </c>
-      <c r="S46">
-        <v>278</v>
-      </c>
-      <c r="T46">
-        <v>521</v>
-      </c>
-      <c r="U46">
-        <v>435</v>
-      </c>
-      <c r="V46">
-        <v>373</v>
-      </c>
-      <c r="W46">
-        <v>2399273</v>
+        <v>2332804</v>
       </c>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
@@ -2593,25 +2572,10 @@
         <v>2304184</v>
       </c>
       <c r="I47">
-        <v>173</v>
+        <v>41080</v>
       </c>
       <c r="J47">
-        <v>365</v>
-      </c>
-      <c r="K47">
-        <v>301</v>
-      </c>
-      <c r="L47">
-        <v>553</v>
-      </c>
-      <c r="M47">
-        <v>431</v>
-      </c>
-      <c r="N47">
-        <v>387</v>
-      </c>
-      <c r="O47">
-        <v>2579139</v>
+        <v>2542945</v>
       </c>
       <c r="Q47">
         <v>128</v>
@@ -2632,7 +2596,7 @@
         <v>373</v>
       </c>
       <c r="W47">
-        <v>2471026</v>
+        <v>2399273</v>
       </c>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
@@ -2658,10 +2622,10 @@
         <v>2375934</v>
       </c>
       <c r="I48">
-        <v>150</v>
+        <v>173</v>
       </c>
       <c r="J48">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="K48">
         <v>301</v>
@@ -2676,13 +2640,28 @@
         <v>387</v>
       </c>
       <c r="O48">
-        <v>2650844</v>
+        <v>2579139</v>
       </c>
       <c r="Q48">
-        <v>161912</v>
+        <v>128</v>
       </c>
       <c r="R48">
-        <v>2495267</v>
+        <v>356</v>
+      </c>
+      <c r="S48">
+        <v>278</v>
+      </c>
+      <c r="T48">
+        <v>521</v>
+      </c>
+      <c r="U48">
+        <v>435</v>
+      </c>
+      <c r="V48">
+        <v>373</v>
+      </c>
+      <c r="W48">
+        <v>2471026</v>
       </c>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
@@ -2693,31 +2672,31 @@
         <v>2440319</v>
       </c>
       <c r="I49">
-        <v>116340</v>
+        <v>150</v>
       </c>
       <c r="J49">
-        <v>2659764</v>
+        <v>362</v>
+      </c>
+      <c r="K49">
+        <v>301</v>
+      </c>
+      <c r="L49">
+        <v>553</v>
+      </c>
+      <c r="M49">
+        <v>431</v>
+      </c>
+      <c r="N49">
+        <v>387</v>
+      </c>
+      <c r="O49">
+        <v>2650844</v>
       </c>
       <c r="Q49">
-        <v>75</v>
+        <v>161912</v>
       </c>
       <c r="R49">
-        <v>339</v>
-      </c>
-      <c r="S49">
-        <v>246</v>
-      </c>
-      <c r="T49">
-        <v>478</v>
-      </c>
-      <c r="U49">
-        <v>435</v>
-      </c>
-      <c r="V49">
-        <v>367</v>
-      </c>
-      <c r="W49">
-        <v>2541728</v>
+        <v>2495267</v>
       </c>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.25">
@@ -2743,16 +2722,31 @@
         <v>2447686</v>
       </c>
       <c r="I50">
-        <v>55472</v>
+        <v>116340</v>
       </c>
       <c r="J50">
-        <v>2715031</v>
+        <v>2659764</v>
       </c>
       <c r="Q50">
-        <v>86600</v>
+        <v>75</v>
       </c>
       <c r="R50">
-        <v>2581709</v>
+        <v>339</v>
+      </c>
+      <c r="S50">
+        <v>246</v>
+      </c>
+      <c r="T50">
+        <v>478</v>
+      </c>
+      <c r="U50">
+        <v>435</v>
+      </c>
+      <c r="V50">
+        <v>367</v>
+      </c>
+      <c r="W50">
+        <v>2541728</v>
       </c>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.25">
@@ -2763,46 +2757,16 @@
         <v>2511050</v>
       </c>
       <c r="I51">
-        <v>150</v>
+        <v>55472</v>
       </c>
       <c r="J51">
-        <v>362</v>
-      </c>
-      <c r="K51">
-        <v>290</v>
-      </c>
-      <c r="L51">
-        <v>538</v>
-      </c>
-      <c r="M51">
-        <v>433</v>
-      </c>
-      <c r="N51">
-        <v>380</v>
-      </c>
-      <c r="O51">
-        <v>2722596</v>
+        <v>2715031</v>
       </c>
       <c r="Q51">
-        <v>60</v>
+        <v>86600</v>
       </c>
       <c r="R51">
-        <v>332</v>
-      </c>
-      <c r="S51">
-        <v>239</v>
-      </c>
-      <c r="T51">
-        <v>468</v>
-      </c>
-      <c r="U51">
-        <v>434</v>
-      </c>
-      <c r="V51">
-        <v>367</v>
-      </c>
-      <c r="W51">
-        <v>2612437</v>
+        <v>2581709</v>
       </c>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.25">
@@ -2828,25 +2792,25 @@
         <v>2519430</v>
       </c>
       <c r="I52">
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="J52">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="K52">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="L52">
-        <v>515</v>
+        <v>538</v>
       </c>
       <c r="M52">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="N52">
-        <v>372</v>
+        <v>380</v>
       </c>
       <c r="O52">
-        <v>2794386</v>
+        <v>2722596</v>
       </c>
       <c r="Q52">
         <v>60</v>
@@ -2867,7 +2831,7 @@
         <v>367</v>
       </c>
       <c r="W52">
-        <v>2683148</v>
+        <v>2612437</v>
       </c>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.25">
@@ -2893,31 +2857,46 @@
         <v>2591182</v>
       </c>
       <c r="I53">
-        <v>135088</v>
+        <v>120</v>
       </c>
       <c r="J53">
-        <v>2850625</v>
+        <v>354</v>
+      </c>
+      <c r="K53">
+        <v>275</v>
+      </c>
+      <c r="L53">
+        <v>515</v>
+      </c>
+      <c r="M53">
+        <v>436</v>
+      </c>
+      <c r="N53">
+        <v>372</v>
+      </c>
+      <c r="O53">
+        <v>2794386</v>
       </c>
       <c r="Q53">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="R53">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="S53">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="T53">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="U53">
         <v>434</v>
       </c>
       <c r="V53">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="W53">
-        <v>2753855</v>
+        <v>2683148</v>
       </c>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.25">
@@ -2943,46 +2922,31 @@
         <v>2662971</v>
       </c>
       <c r="I54">
-        <v>120</v>
+        <v>135088</v>
       </c>
       <c r="J54">
-        <v>354</v>
-      </c>
-      <c r="K54">
-        <v>275</v>
-      </c>
-      <c r="L54">
-        <v>515</v>
-      </c>
-      <c r="M54">
-        <v>436</v>
-      </c>
-      <c r="N54">
-        <v>372</v>
-      </c>
-      <c r="O54">
-        <v>2866092</v>
+        <v>2850625</v>
       </c>
       <c r="Q54">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="R54">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="S54">
         <v>242</v>
       </c>
       <c r="T54">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="U54">
         <v>434</v>
       </c>
       <c r="V54">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="W54">
-        <v>2824606</v>
+        <v>2753855</v>
       </c>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.25">
@@ -2993,16 +2957,46 @@
         <v>2696130</v>
       </c>
       <c r="I55">
-        <v>62364</v>
+        <v>120</v>
       </c>
       <c r="J55">
-        <v>2912797</v>
+        <v>354</v>
+      </c>
+      <c r="K55">
+        <v>275</v>
+      </c>
+      <c r="L55">
+        <v>515</v>
+      </c>
+      <c r="M55">
+        <v>436</v>
+      </c>
+      <c r="N55">
+        <v>372</v>
+      </c>
+      <c r="O55">
+        <v>2866092</v>
       </c>
       <c r="Q55">
-        <v>252804</v>
+        <v>65</v>
       </c>
       <c r="R55">
-        <v>2835210</v>
+        <v>335</v>
+      </c>
+      <c r="S55">
+        <v>242</v>
+      </c>
+      <c r="T55">
+        <v>472</v>
+      </c>
+      <c r="U55">
+        <v>434</v>
+      </c>
+      <c r="V55">
+        <v>367</v>
+      </c>
+      <c r="W55">
+        <v>2824606</v>
       </c>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.25">
@@ -3028,46 +3022,16 @@
         <v>2734679</v>
       </c>
       <c r="I56">
-        <v>80</v>
+        <v>62364</v>
       </c>
       <c r="J56">
-        <v>341</v>
-      </c>
-      <c r="K56">
-        <v>249</v>
-      </c>
-      <c r="L56">
-        <v>483</v>
-      </c>
-      <c r="M56">
-        <v>435</v>
-      </c>
-      <c r="N56">
-        <v>368</v>
-      </c>
-      <c r="O56">
-        <v>2936794</v>
+        <v>2912797</v>
       </c>
       <c r="Q56">
-        <v>65</v>
+        <v>252804</v>
       </c>
       <c r="R56">
-        <v>335</v>
-      </c>
-      <c r="S56">
-        <v>242</v>
-      </c>
-      <c r="T56">
-        <v>472</v>
-      </c>
-      <c r="U56">
-        <v>434</v>
-      </c>
-      <c r="V56">
-        <v>367</v>
-      </c>
-      <c r="W56">
-        <v>2895316</v>
+        <v>2835210</v>
       </c>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.25">
@@ -3078,25 +3042,25 @@
         <v>2793198</v>
       </c>
       <c r="I57">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="J57">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="K57">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="L57">
-        <v>469</v>
+        <v>483</v>
       </c>
       <c r="M57">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="N57">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="O57">
-        <v>3007504</v>
+        <v>2936794</v>
       </c>
       <c r="Q57">
         <v>65</v>
@@ -3105,19 +3069,19 @@
         <v>335</v>
       </c>
       <c r="S57">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="T57">
         <v>472</v>
       </c>
       <c r="U57">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V57">
         <v>367</v>
       </c>
       <c r="W57">
-        <v>2966027</v>
+        <v>2895316</v>
       </c>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.25">
@@ -3161,7 +3125,7 @@
         <v>367</v>
       </c>
       <c r="O58">
-        <v>3078215</v>
+        <v>3007504</v>
       </c>
       <c r="Q58">
         <v>65</v>
@@ -3182,7 +3146,7 @@
         <v>367</v>
       </c>
       <c r="W58">
-        <v>3036735</v>
+        <v>2966027</v>
       </c>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.25">
@@ -3208,16 +3172,46 @@
         <v>2878221</v>
       </c>
       <c r="I59">
-        <v>192556</v>
+        <v>62</v>
       </c>
       <c r="J59">
-        <v>3105950</v>
+        <v>334</v>
+      </c>
+      <c r="K59">
+        <v>239</v>
+      </c>
+      <c r="L59">
+        <v>469</v>
+      </c>
+      <c r="M59">
+        <v>434</v>
+      </c>
+      <c r="N59">
+        <v>367</v>
+      </c>
+      <c r="O59">
+        <v>3078215</v>
       </c>
       <c r="Q59">
-        <v>239428</v>
+        <v>65</v>
       </c>
       <c r="R59">
-        <v>3075014</v>
+        <v>335</v>
+      </c>
+      <c r="S59">
+        <v>241</v>
+      </c>
+      <c r="T59">
+        <v>472</v>
+      </c>
+      <c r="U59">
+        <v>435</v>
+      </c>
+      <c r="V59">
+        <v>367</v>
+      </c>
+      <c r="W59">
+        <v>3036735</v>
       </c>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.25">
@@ -3243,31 +3237,16 @@
         <v>2949925</v>
       </c>
       <c r="I60">
-        <v>62</v>
+        <v>192556</v>
       </c>
       <c r="J60">
-        <v>334</v>
-      </c>
-      <c r="K60">
-        <v>239</v>
-      </c>
-      <c r="L60">
-        <v>469</v>
-      </c>
-      <c r="M60">
-        <v>434</v>
-      </c>
-      <c r="N60">
-        <v>367</v>
-      </c>
-      <c r="O60">
-        <v>3148923</v>
+        <v>3105950</v>
       </c>
       <c r="Q60">
-        <v>340</v>
+        <v>239428</v>
       </c>
       <c r="R60">
-        <v>3076314</v>
+        <v>3075014</v>
       </c>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.25">
@@ -3293,7 +3272,7 @@
         <v>3021678</v>
       </c>
       <c r="I61">
-        <v>162</v>
+        <v>62</v>
       </c>
       <c r="J61">
         <v>334</v>
@@ -3311,13 +3290,13 @@
         <v>367</v>
       </c>
       <c r="O61">
-        <v>3219634</v>
+        <v>3148923</v>
       </c>
       <c r="Q61">
-        <v>212</v>
+        <v>340</v>
       </c>
       <c r="R61">
-        <v>3077616</v>
+        <v>3076314</v>
       </c>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.25">
@@ -3343,16 +3322,31 @@
         <v>3093467</v>
       </c>
       <c r="I62">
-        <v>14864</v>
+        <v>162</v>
       </c>
       <c r="J62">
-        <v>3220996</v>
+        <v>334</v>
+      </c>
+      <c r="K62">
+        <v>239</v>
+      </c>
+      <c r="L62">
+        <v>469</v>
+      </c>
+      <c r="M62">
+        <v>434</v>
+      </c>
+      <c r="N62">
+        <v>367</v>
+      </c>
+      <c r="O62">
+        <v>3219634</v>
       </c>
       <c r="Q62">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="R62">
-        <v>3078920</v>
+        <v>3077616</v>
       </c>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.25">
@@ -3378,31 +3372,16 @@
         <v>3165176</v>
       </c>
       <c r="I63">
-        <v>62</v>
+        <v>14864</v>
       </c>
       <c r="J63">
-        <v>334</v>
-      </c>
-      <c r="K63">
-        <v>239</v>
-      </c>
-      <c r="L63">
-        <v>469</v>
-      </c>
-      <c r="M63">
-        <v>434</v>
-      </c>
-      <c r="N63">
-        <v>367</v>
-      </c>
-      <c r="O63">
-        <v>3290343</v>
+        <v>3220996</v>
       </c>
       <c r="Q63">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="R63">
-        <v>3080220</v>
+        <v>3078920</v>
       </c>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.25">
@@ -3446,13 +3425,13 @@
         <v>367</v>
       </c>
       <c r="O64">
-        <v>3361093</v>
+        <v>3290343</v>
       </c>
       <c r="Q64">
-        <v>340</v>
+        <v>204</v>
       </c>
       <c r="R64">
-        <v>3081524</v>
+        <v>3080220</v>
       </c>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.25">
@@ -3496,13 +3475,13 @@
         <v>367</v>
       </c>
       <c r="O65">
-        <v>3431801</v>
+        <v>3361093</v>
       </c>
       <c r="Q65">
-        <v>208</v>
+        <v>340</v>
       </c>
       <c r="R65">
-        <v>3082824</v>
+        <v>3081524</v>
       </c>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.25">
@@ -3546,13 +3525,13 @@
         <v>367</v>
       </c>
       <c r="O66">
-        <v>3502511</v>
+        <v>3431801</v>
       </c>
       <c r="Q66">
-        <v>236</v>
+        <v>208</v>
       </c>
       <c r="R66">
-        <v>3084127</v>
+        <v>3082824</v>
       </c>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.25">
@@ -3578,7 +3557,7 @@
         <v>3452175</v>
       </c>
       <c r="I67">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J67">
         <v>334</v>
@@ -3596,13 +3575,13 @@
         <v>367</v>
       </c>
       <c r="O67">
-        <v>3573222</v>
+        <v>3502511</v>
       </c>
       <c r="Q67">
-        <v>208</v>
+        <v>236</v>
       </c>
       <c r="R67">
-        <v>3087521</v>
+        <v>3084127</v>
       </c>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.25">
@@ -3646,13 +3625,13 @@
         <v>367</v>
       </c>
       <c r="O68">
-        <v>3643886</v>
+        <v>3573222</v>
       </c>
       <c r="Q68">
-        <v>688</v>
+        <v>208</v>
       </c>
       <c r="R68">
-        <v>3091168</v>
+        <v>3087521</v>
       </c>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.25">
@@ -3696,13 +3675,13 @@
         <v>367</v>
       </c>
       <c r="O69">
-        <v>3714596</v>
+        <v>3643886</v>
       </c>
       <c r="Q69">
-        <v>200</v>
+        <v>688</v>
       </c>
       <c r="R69">
-        <v>3094813</v>
+        <v>3091168</v>
       </c>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.25">
@@ -3737,7 +3716,7 @@
         <v>239</v>
       </c>
       <c r="L70">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="M70">
         <v>434</v>
@@ -3746,28 +3725,13 @@
         <v>367</v>
       </c>
       <c r="O70">
-        <v>3785306</v>
+        <v>3714596</v>
       </c>
       <c r="Q70">
-        <v>65</v>
+        <v>200</v>
       </c>
       <c r="R70">
-        <v>335</v>
-      </c>
-      <c r="S70">
-        <v>241</v>
-      </c>
-      <c r="T70">
-        <v>472</v>
-      </c>
-      <c r="U70">
-        <v>435</v>
-      </c>
-      <c r="V70">
-        <v>367</v>
-      </c>
-      <c r="W70">
-        <v>3107400</v>
+        <v>3094813</v>
       </c>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.25">
@@ -3811,7 +3775,7 @@
         <v>367</v>
       </c>
       <c r="O71">
-        <v>3856016</v>
+        <v>3785306</v>
       </c>
       <c r="Q71">
         <v>65</v>
@@ -3826,13 +3790,13 @@
         <v>472</v>
       </c>
       <c r="U71">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="V71">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="W71">
-        <v>3178110</v>
+        <v>3107400</v>
       </c>
     </row>
     <row r="72" spans="1:23" x14ac:dyDescent="0.25">
@@ -3876,7 +3840,7 @@
         <v>367</v>
       </c>
       <c r="O72">
-        <v>3926726</v>
+        <v>3856016</v>
       </c>
       <c r="Q72">
         <v>65</v>
@@ -3897,7 +3861,7 @@
         <v>368</v>
       </c>
       <c r="W72">
-        <v>3248819</v>
+        <v>3178110</v>
       </c>
     </row>
     <row r="73" spans="1:23" x14ac:dyDescent="0.25">
@@ -3935,13 +3899,13 @@
         <v>468</v>
       </c>
       <c r="M73">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="N73">
         <v>367</v>
       </c>
       <c r="O73">
-        <v>3997435</v>
+        <v>3926726</v>
       </c>
       <c r="Q73">
         <v>65</v>
@@ -3953,16 +3917,16 @@
         <v>241</v>
       </c>
       <c r="T73">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="U73">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V73">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="W73">
-        <v>3319529</v>
+        <v>3248819</v>
       </c>
     </row>
     <row r="74" spans="1:23" x14ac:dyDescent="0.25">
@@ -3985,7 +3949,7 @@
         <v>367</v>
       </c>
       <c r="O74">
-        <v>4068144</v>
+        <v>3997435</v>
       </c>
       <c r="Q74">
         <v>65</v>
@@ -3997,16 +3961,16 @@
         <v>241</v>
       </c>
       <c r="T74">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="U74">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="V74">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="W74">
-        <v>3390240</v>
+        <v>3319529</v>
       </c>
     </row>
     <row r="75" spans="1:23" x14ac:dyDescent="0.25">
@@ -4023,13 +3987,13 @@
         <v>468</v>
       </c>
       <c r="M75">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="N75">
         <v>367</v>
       </c>
       <c r="O75">
-        <v>4138855</v>
+        <v>4068144</v>
       </c>
       <c r="Q75">
         <v>65</v>
@@ -4050,7 +4014,7 @@
         <v>368</v>
       </c>
       <c r="W75">
-        <v>3460950</v>
+        <v>3390240</v>
       </c>
     </row>
     <row r="76" spans="1:23" x14ac:dyDescent="0.25">
@@ -4058,7 +4022,7 @@
         <v>61</v>
       </c>
       <c r="J76">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="K76">
         <v>239</v>
@@ -4073,7 +4037,7 @@
         <v>367</v>
       </c>
       <c r="O76">
-        <v>4209564</v>
+        <v>4138855</v>
       </c>
       <c r="Q76">
         <v>65</v>
@@ -4085,16 +4049,16 @@
         <v>241</v>
       </c>
       <c r="T76">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="U76">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V76">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="W76">
-        <v>3531658</v>
+        <v>3460950</v>
       </c>
     </row>
     <row r="77" spans="1:23" x14ac:dyDescent="0.25">
@@ -4117,7 +4081,7 @@
         <v>367</v>
       </c>
       <c r="O77">
-        <v>4280275</v>
+        <v>4209564</v>
       </c>
       <c r="Q77">
         <v>65</v>
@@ -4129,16 +4093,16 @@
         <v>241</v>
       </c>
       <c r="T77">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="U77">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="V77">
         <v>367</v>
       </c>
       <c r="W77">
-        <v>3602369</v>
+        <v>3531658</v>
       </c>
     </row>
     <row r="78" spans="1:23" x14ac:dyDescent="0.25">
@@ -4161,7 +4125,7 @@
         <v>367</v>
       </c>
       <c r="O78">
-        <v>4351024</v>
+        <v>4280275</v>
       </c>
       <c r="Q78">
         <v>65</v>
@@ -4182,7 +4146,7 @@
         <v>367</v>
       </c>
       <c r="W78">
-        <v>3673078</v>
+        <v>3602369</v>
       </c>
     </row>
     <row r="79" spans="1:23" x14ac:dyDescent="0.25">
@@ -4205,7 +4169,7 @@
         <v>367</v>
       </c>
       <c r="O79">
-        <v>4421732</v>
+        <v>4351024</v>
       </c>
       <c r="Q79">
         <v>65</v>
@@ -4217,16 +4181,16 @@
         <v>241</v>
       </c>
       <c r="T79">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="U79">
         <v>434</v>
       </c>
       <c r="V79">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="W79">
-        <v>3743789</v>
+        <v>3673078</v>
       </c>
     </row>
     <row r="80" spans="1:23" x14ac:dyDescent="0.25">
@@ -4240,7 +4204,7 @@
         <v>239</v>
       </c>
       <c r="L80">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="M80">
         <v>434</v>
@@ -4249,7 +4213,7 @@
         <v>367</v>
       </c>
       <c r="O80">
-        <v>4492443</v>
+        <v>4421732</v>
       </c>
       <c r="Q80">
         <v>65</v>
@@ -4270,7 +4234,7 @@
         <v>368</v>
       </c>
       <c r="W80">
-        <v>3814537</v>
+        <v>3743789</v>
       </c>
     </row>
     <row r="81" spans="9:23" x14ac:dyDescent="0.25">
@@ -4284,7 +4248,7 @@
         <v>239</v>
       </c>
       <c r="L81">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="M81">
         <v>434</v>
@@ -4293,7 +4257,7 @@
         <v>367</v>
       </c>
       <c r="O81">
-        <v>4563151</v>
+        <v>4492443</v>
       </c>
       <c r="Q81">
         <v>65</v>
@@ -4314,7 +4278,7 @@
         <v>368</v>
       </c>
       <c r="W81">
-        <v>3885248</v>
+        <v>3814537</v>
       </c>
     </row>
     <row r="82" spans="9:23" x14ac:dyDescent="0.25">
@@ -4337,7 +4301,7 @@
         <v>367</v>
       </c>
       <c r="O82">
-        <v>4633817</v>
+        <v>4563151</v>
       </c>
       <c r="Q82">
         <v>65</v>
@@ -4349,7 +4313,7 @@
         <v>241</v>
       </c>
       <c r="T82">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="U82">
         <v>434</v>
@@ -4358,7 +4322,7 @@
         <v>368</v>
       </c>
       <c r="W82">
-        <v>3955957</v>
+        <v>3885248</v>
       </c>
     </row>
     <row r="83" spans="9:23" x14ac:dyDescent="0.25">
@@ -4381,7 +4345,7 @@
         <v>367</v>
       </c>
       <c r="O83">
-        <v>4704526</v>
+        <v>4633817</v>
       </c>
       <c r="Q83">
         <v>65</v>
@@ -4402,7 +4366,7 @@
         <v>368</v>
       </c>
       <c r="W83">
-        <v>4026666</v>
+        <v>3955957</v>
       </c>
     </row>
     <row r="84" spans="9:23" x14ac:dyDescent="0.25">
@@ -4416,7 +4380,7 @@
         <v>239</v>
       </c>
       <c r="L84">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="M84">
         <v>434</v>
@@ -4425,7 +4389,7 @@
         <v>367</v>
       </c>
       <c r="O84">
-        <v>4775235</v>
+        <v>4704526</v>
       </c>
       <c r="Q84">
         <v>65</v>
@@ -4437,7 +4401,7 @@
         <v>241</v>
       </c>
       <c r="T84">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="U84">
         <v>434</v>
@@ -4446,10 +4410,31 @@
         <v>368</v>
       </c>
       <c r="W84">
-        <v>4097331</v>
+        <v>4026666</v>
       </c>
     </row>
     <row r="85" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <v>61</v>
+      </c>
+      <c r="J85">
+        <v>333</v>
+      </c>
+      <c r="K85">
+        <v>239</v>
+      </c>
+      <c r="L85">
+        <v>467</v>
+      </c>
+      <c r="M85">
+        <v>434</v>
+      </c>
+      <c r="N85">
+        <v>367</v>
+      </c>
+      <c r="O85">
+        <v>4775235</v>
+      </c>
       <c r="Q85">
         <v>65</v>
       </c>
@@ -4460,16 +4445,16 @@
         <v>241</v>
       </c>
       <c r="T85">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="U85">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="V85">
         <v>368</v>
       </c>
       <c r="W85">
-        <v>4168041</v>
+        <v>4097331</v>
       </c>
     </row>
     <row r="86" spans="9:23" x14ac:dyDescent="0.25">
@@ -4492,7 +4477,7 @@
         <v>368</v>
       </c>
       <c r="W86">
-        <v>4238750</v>
+        <v>4168041</v>
       </c>
     </row>
     <row r="87" spans="9:23" x14ac:dyDescent="0.25">
@@ -4506,16 +4491,16 @@
         <v>241</v>
       </c>
       <c r="T87">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="U87">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="V87">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="W87">
-        <v>4309460</v>
+        <v>4238750</v>
       </c>
     </row>
     <row r="88" spans="9:23" x14ac:dyDescent="0.25">
@@ -4532,12 +4517,35 @@
         <v>471</v>
       </c>
       <c r="U88">
+        <v>434</v>
+      </c>
+      <c r="V88">
+        <v>367</v>
+      </c>
+      <c r="W88">
+        <v>4309460</v>
+      </c>
+    </row>
+    <row r="89" spans="9:23" x14ac:dyDescent="0.25">
+      <c r="Q89">
+        <v>65</v>
+      </c>
+      <c r="R89">
+        <v>335</v>
+      </c>
+      <c r="S89">
+        <v>241</v>
+      </c>
+      <c r="T89">
+        <v>471</v>
+      </c>
+      <c r="U89">
         <v>435</v>
       </c>
-      <c r="V88">
+      <c r="V89">
         <v>368</v>
       </c>
-      <c r="W88">
+      <c r="W89">
         <v>4380171</v>
       </c>
     </row>
@@ -4551,7 +4559,7 @@
   <dimension ref="A1:W68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:W64"/>
+      <selection activeCell="G1" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7879,7 +7887,7 @@
   <dimension ref="A1:W86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:W85"/>
+      <selection activeCell="G1" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12052,8 +12060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AA81B26-3000-48E8-869A-8BF2E6686498}">
   <dimension ref="A1:W106"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1048576"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G34" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16720,8 +16728,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F38D4CC7-A132-4103-9F53-3F4842909E33}">
   <dimension ref="A1:W91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:W72"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="G64" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20916,8 +20924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B394E29-286A-4D6B-95F0-F8C2EF83229A}">
   <dimension ref="A1:W99"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:W80"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>